<commit_message>
Add logic for Sensor's settings
</commit_message>
<xml_diff>
--- a/struct.xlsx
+++ b/struct.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Roman\Documents\Arduino\ESP32_HTTPS_OTA_APT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46ADBEF0-1429-4777-8B57-5BBBF727CFE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85D5FC58-87DA-4EB2-BC06-B143DD8E4124}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{40B8887A-0BD1-4A86-807F-5934227B243E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{40B8887A-0BD1-4A86-807F-5934227B243E}"/>
   </bookViews>
   <sheets>
     <sheet name="Struct" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="API" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Struct!$B$1:$E$79</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Struct!$B$1:$E$76</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="273">
   <si>
     <t>doc["r_en"]</t>
   </si>
@@ -127,12 +127,6 @@
     <t>config.nodes.climate.bme280.enabled</t>
   </si>
   <si>
-    <t>config.nodes.climate.bme280.type</t>
-  </si>
-  <si>
-    <t>"I2C"</t>
-  </si>
-  <si>
     <t>config.nodes.climate.bme280.labels</t>
   </si>
   <si>
@@ -163,15 +157,6 @@
     <t>config.nodes.climate.dht22.enabled</t>
   </si>
   <si>
-    <t>config.nodes.climate.dht22.pins</t>
-  </si>
-  <si>
-    <t>[4]</t>
-  </si>
-  <si>
-    <t>[15]</t>
-  </si>
-  <si>
     <t>config.nodes.climate.dht22.labels</t>
   </si>
   <si>
@@ -199,9 +184,6 @@
     <t>config.nodes.climate.ds18b20.enabled</t>
   </si>
   <si>
-    <t>config.nodes.climate.ds18b20.pins</t>
-  </si>
-  <si>
     <t>["", "", "", ""]</t>
   </si>
   <si>
@@ -214,9 +196,6 @@
     <t>config.nodes.climate.ds18b20.units</t>
   </si>
   <si>
-    <t>["°C"]</t>
-  </si>
-  <si>
     <t>config.nodes.climate.ds18b20.ui_cards</t>
   </si>
   <si>
@@ -232,12 +211,6 @@
     <t>config.nodes.binary.pir.pin</t>
   </si>
   <si>
-    <t>config.nodes.binary.pir.type</t>
-  </si>
-  <si>
-    <t>"motion"</t>
-  </si>
-  <si>
     <t>config.nodes.binary.pir.label</t>
   </si>
   <si>
@@ -262,9 +235,6 @@
     <t>config.nodes.binary.ld2420.pin</t>
   </si>
   <si>
-    <t>config.nodes.binary.ld2420.type</t>
-  </si>
-  <si>
     <t>config.nodes.binary.ld2420.label</t>
   </si>
   <si>
@@ -274,9 +244,6 @@
     <t>config.nodes.binary.ld2420.topic</t>
   </si>
   <si>
-    <t>"presence"</t>
-  </si>
-  <si>
     <t>"Присутствие"</t>
   </si>
   <si>
@@ -322,9 +289,6 @@
     <t>config.nodes.binary.flood.pin</t>
   </si>
   <si>
-    <t>config.nodes.binary.flood.type</t>
-  </si>
-  <si>
     <t>config.nodes.binary.flood.label</t>
   </si>
   <si>
@@ -334,9 +298,6 @@
     <t>config.nodes.binary.flood.topic</t>
   </si>
   <si>
-    <t>"leak"</t>
-  </si>
-  <si>
     <t>"Затопление"</t>
   </si>
   <si>
@@ -370,33 +331,9 @@
     <t>config.nodes.climate.tcrt5000.enabled</t>
   </si>
   <si>
-    <t>config.nodes.climate.tcrt5000.type</t>
-  </si>
-  <si>
-    <t>config.nodes.climate.tcrt5000.labels</t>
-  </si>
-  <si>
-    <t>config.nodes.climate.tcrt5000.units</t>
-  </si>
-  <si>
-    <t>config.nodes.climate.tcrt5000.ui_cards</t>
-  </si>
-  <si>
-    <t>config.nodes.climate.tcrt5000.topics</t>
-  </si>
-  <si>
     <t>["Освещение (TCRT)"]</t>
   </si>
   <si>
-    <t>["Lux"]</t>
-  </si>
-  <si>
-    <t>["card-tcrt"]</t>
-  </si>
-  <si>
-    <t>["/lux"]</t>
-  </si>
-  <si>
     <t>"/lux_raw"</t>
   </si>
   <si>
@@ -481,9 +418,6 @@
     <t>doc["bme_c"]</t>
   </si>
   <si>
-    <t>doc["bme_type"]</t>
-  </si>
-  <si>
     <t>doc["dht_en"]</t>
   </si>
   <si>
@@ -544,15 +478,6 @@
     <t>doc["door_en"]</t>
   </si>
   <si>
-    <t>doc["tcrt_type"]</t>
-  </si>
-  <si>
-    <t>doc["pir_type"]</t>
-  </si>
-  <si>
-    <t>doc["ld_type"]</t>
-  </si>
-  <si>
     <t>doc["door_type"]</t>
   </si>
   <si>
@@ -598,9 +523,6 @@
     <t>doc["fl_p"]</t>
   </si>
   <si>
-    <t>doc["fl_type"]</t>
-  </si>
-  <si>
     <t>doc["fl_l"]</t>
   </si>
   <si>
@@ -637,21 +559,12 @@
     <t>doc["r_t"]</t>
   </si>
   <si>
-    <t>doc["s_ssid"]</t>
-  </si>
-  <si>
-    <t>doc["s_pass"]</t>
-  </si>
-  <si>
     <t>doc["s_rbi"]</t>
   </si>
   <si>
     <t>doc["s_dn"]</t>
   </si>
   <si>
-    <t>doc["s_ap"]</t>
-  </si>
-  <si>
     <t>doc["u_l"]</t>
   </si>
   <si>
@@ -736,9 +649,6 @@
     <t>char type[8]</t>
   </si>
   <si>
-    <t>char type[12]</t>
-  </si>
-  <si>
     <t>char labels[3][32]</t>
   </si>
   <si>
@@ -748,9 +658,6 @@
     <t>char topics[3][16]</t>
   </si>
   <si>
-    <t>int pins[1]</t>
-  </si>
-  <si>
     <t>int pins[4]</t>
   </si>
   <si>
@@ -778,39 +685,15 @@
     <t>char ui_cards[3][16]</t>
   </si>
   <si>
-    <t>char units[1][8]</t>
-  </si>
-  <si>
     <t>ui_cards[2][16]</t>
   </si>
   <si>
-    <t>char type[4]</t>
-  </si>
-  <si>
-    <t>char labels[1][32]</t>
-  </si>
-  <si>
-    <t>char ui_cards[1][16]</t>
-  </si>
-  <si>
-    <t>char topics[1][16]</t>
-  </si>
-  <si>
     <t>char topic[16]</t>
   </si>
   <si>
     <t>char ui_card[16]</t>
   </si>
   <si>
-    <t>doc["5516_type"]</t>
-  </si>
-  <si>
-    <t>config.nodes.analog.light_resistor.type</t>
-  </si>
-  <si>
-    <t>"light"</t>
-  </si>
-  <si>
     <t>char topics[[4][16]</t>
   </si>
   <si>
@@ -911,6 +794,75 @@
   </si>
   <si>
     <t>получение настроек</t>
+  </si>
+  <si>
+    <t>doc["w_en"]</t>
+  </si>
+  <si>
+    <t>doc["w_ssid"]</t>
+  </si>
+  <si>
+    <t>doc["w_pass"]</t>
+  </si>
+  <si>
+    <t>doc["w_ap"]</t>
+  </si>
+  <si>
+    <t>config.services.wifi.enabled</t>
+  </si>
+  <si>
+    <t>doc["bme_p"]</t>
+  </si>
+  <si>
+    <t>config.nodes.climate.bme280.pin</t>
+  </si>
+  <si>
+    <t>doc["tcrt_p"]</t>
+  </si>
+  <si>
+    <t>config.nodes.climate.tcrt5000.pin</t>
+  </si>
+  <si>
+    <t>config.nodes.climate.dht22.pin</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>21/22, "I2C"</t>
+  </si>
+  <si>
+    <t>char units[4][8]</t>
+  </si>
+  <si>
+    <t>["°C","°C","°C","°C"]</t>
+  </si>
+  <si>
+    <t>config.nodes.climate.ds18b20.pin</t>
+  </si>
+  <si>
+    <t>char unit[8]</t>
+  </si>
+  <si>
+    <t>"Lux"</t>
+  </si>
+  <si>
+    <t>"card-tcrt"</t>
+  </si>
+  <si>
+    <t>"/lux"</t>
+  </si>
+  <si>
+    <t>config.nodes.climate.tcrt5000.ui_card</t>
+  </si>
+  <si>
+    <t>config.nodes.climate.tcrt5000.topic</t>
+  </si>
+  <si>
+    <t>config.nodes.climate.tcrt5000.unit</t>
+  </si>
+  <si>
+    <t>config.nodes.climate.tcrt5000.label</t>
   </si>
 </sst>
 </file>
@@ -1344,10 +1296,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16B76558-8B24-41A2-80CE-D2D9E66F99DE}">
-  <dimension ref="A1:F79"/>
+  <dimension ref="A1:F76"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C61" sqref="C61"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1368,10 +1320,10 @@
         <v>3</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>213</v>
+        <v>184</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>131</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1379,13 +1331,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>200</v>
+        <v>172</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>207</v>
+        <v>178</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>4</v>
@@ -1396,13 +1348,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>199</v>
+        <v>171</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>214</v>
+        <v>185</v>
       </c>
       <c r="E3" s="3">
         <v>0</v>
@@ -1410,774 +1362,774 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>197</v>
+        <v>250</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>7</v>
+        <v>254</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>208</v>
+        <v>191</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>218</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>198</v>
+        <v>251</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>216</v>
+        <v>179</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>218</v>
+        <v>189</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>201</v>
+        <v>252</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>217</v>
+        <v>187</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" t="s">
-        <v>118</v>
+        <v>189</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>219</v>
+        <v>5</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>203</v>
+        <v>173</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>209</v>
+        <v>181</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>219</v>
+        <v>190</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>220</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>14</v>
+        <v>7</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>204</v>
+        <v>112</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>221</v>
+        <v>191</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>218</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>205</v>
+        <v>175</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>132</v>
+        <v>15</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>222</v>
-      </c>
-      <c r="E11" s="5">
-        <v>0</v>
+        <v>192</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>206</v>
+        <v>176</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>16</v>
+        <v>111</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>256</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>17</v>
+        <v>193</v>
+      </c>
+      <c r="E12" s="5">
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>135</v>
+        <v>113</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>225</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>136</v>
+        <v>114</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="E15" s="3">
-        <v>1883</v>
+        <v>182</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>226</v>
+        <v>194</v>
+      </c>
+      <c r="E16" s="3">
+        <v>1883</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>138</v>
+        <v>116</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>209</v>
+        <v>181</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>227</v>
+        <v>197</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>257</v>
+        <v>117</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>228</v>
+        <v>180</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F18" t="s">
-        <v>119</v>
+        <v>198</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>139</v>
+        <v>218</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="E19" s="3">
-        <v>5</v>
+        <v>199</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="F19" t="s">
-        <v>120</v>
+        <v>98</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>220</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>14</v>
+        <v>18</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="E20" s="3">
+        <v>5</v>
+      </c>
+      <c r="F20" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>145</v>
+        <v>119</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>246</v>
+        <v>191</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>142</v>
+        <v>255</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>29</v>
+        <v>256</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>231</v>
+        <v>260</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>30</v>
+        <v>261</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>143</v>
+        <v>121</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>232</v>
+        <v>201</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>243</v>
+        <v>202</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>141</v>
+        <v>123</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>233</v>
+        <v>212</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="F25" t="s">
-        <v>121</v>
+        <v>32</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>25</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>14</v>
+        <v>24</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F26" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>147</v>
+        <v>124</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>234</v>
+        <v>191</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>148</v>
+        <v>125</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>42</v>
+        <v>259</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>43</v>
+        <v>195</v>
+      </c>
+      <c r="E28" s="3">
+        <v>15</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>149</v>
+        <v>126</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>237</v>
+        <v>205</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>150</v>
+        <v>127</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>245</v>
+        <v>206</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>154</v>
+        <v>128</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>238</v>
+        <v>213</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F31" t="s">
-        <v>121</v>
+        <v>42</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>31</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>220</v>
-      </c>
-      <c r="E32" s="5" t="s">
-        <v>14</v>
+        <v>30</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F32" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>151</v>
+        <v>133</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>234</v>
+        <v>191</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>40</v>
+        <v>14</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>258</v>
+        <v>129</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>259</v>
+        <v>264</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>239</v>
-      </c>
-      <c r="E34" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="F34" t="s">
-        <v>122</v>
+        <v>195</v>
+      </c>
+      <c r="E34" s="5">
+        <v>4</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>152</v>
+        <v>219</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>53</v>
+        <v>220</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>240</v>
+        <v>208</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>54</v>
+        <v>46</v>
+      </c>
+      <c r="F35" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>153</v>
+        <v>130</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>244</v>
+        <v>209</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>156</v>
+        <v>131</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>241</v>
+        <v>262</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>58</v>
+        <v>263</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>157</v>
+        <v>134</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>242</v>
+        <v>210</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="F38" t="s">
-        <v>121</v>
+        <v>51</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>38</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="E39" s="3" t="s">
-        <v>14</v>
+        <v>37</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F39" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>166</v>
+        <v>136</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>246</v>
+        <v>191</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>159</v>
+        <v>257</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>109</v>
+        <v>258</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>247</v>
+        <v>260</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>113</v>
+        <v>261</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>160</v>
+        <v>137</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>110</v>
+        <v>272</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>244</v>
+        <v>183</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>161</v>
+        <v>138</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>111</v>
+        <v>271</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>248</v>
+        <v>265</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>115</v>
+        <v>266</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>162</v>
+        <v>139</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>112</v>
+        <v>269</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>249</v>
+        <v>215</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="F44" t="s">
-        <v>121</v>
+        <v>267</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>44</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D45" s="4" t="s">
-        <v>220</v>
-      </c>
-      <c r="E45" s="5" t="s">
-        <v>14</v>
+        <v>43</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="F45" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>170</v>
+        <v>141</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>224</v>
-      </c>
-      <c r="E46" s="5">
-        <v>35</v>
+        <v>191</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>167</v>
+        <v>145</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="E47" s="5" t="s">
-        <v>63</v>
+        <v>195</v>
+      </c>
+      <c r="E47" s="5">
+        <v>35</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -2185,16 +2137,16 @@
         <v>47</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>172</v>
+        <v>147</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>212</v>
+        <v>183</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -2202,16 +2154,16 @@
         <v>48</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>174</v>
+        <v>149</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>251</v>
+        <v>215</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -2219,19 +2171,19 @@
         <v>49</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>176</v>
+        <v>151</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>250</v>
+        <v>214</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="F50" t="s">
-        <v>121</v>
+        <v>100</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -2239,13 +2191,13 @@
         <v>50</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>164</v>
+        <v>142</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>220</v>
+        <v>191</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>14</v>
@@ -2256,13 +2208,13 @@
         <v>51</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>178</v>
+        <v>153</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>224</v>
+        <v>195</v>
       </c>
       <c r="E52" s="3">
         <v>35</v>
@@ -2270,480 +2222,429 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>230</v>
+        <v>183</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>179</v>
+        <v>155</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>180</v>
+        <v>156</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>251</v>
+        <v>214</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>78</v>
+        <v>68</v>
+      </c>
+      <c r="F55" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>55</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="E56" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="F56" t="s">
-        <v>121</v>
+        <v>56</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D56" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="E56" s="5" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>165</v>
+        <v>146</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>220</v>
-      </c>
-      <c r="E57" s="5" t="s">
-        <v>14</v>
+        <v>195</v>
+      </c>
+      <c r="E57" s="5">
+        <v>36</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>171</v>
+        <v>144</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>224</v>
-      </c>
-      <c r="E58" s="5">
-        <v>36</v>
+        <v>200</v>
+      </c>
+      <c r="E58" s="5" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>169</v>
+        <v>148</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>229</v>
+        <v>183</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>173</v>
+        <v>150</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="E60" s="5" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>175</v>
+        <v>152</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>251</v>
+        <v>214</v>
       </c>
       <c r="E61" s="5" t="s">
-        <v>88</v>
+        <v>78</v>
+      </c>
+      <c r="F61" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>61</v>
-      </c>
-      <c r="B62" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="C62" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="D62" s="4" t="s">
-        <v>250</v>
-      </c>
-      <c r="E62" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="F62" t="s">
-        <v>121</v>
+        <v>62</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>182</v>
+        <v>158</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="E63" s="3" t="s">
-        <v>14</v>
+        <v>195</v>
+      </c>
+      <c r="E63" s="3">
+        <v>34</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B64" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D64" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="C64" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="D64" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="E64" s="3">
-        <v>34</v>
+      <c r="E64" s="3" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>184</v>
+        <v>160</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>229</v>
+        <v>215</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>185</v>
+        <v>161</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>97</v>
+        <v>86</v>
+      </c>
+      <c r="F66" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>66</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="C67" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="D67" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="E67" s="3" t="s">
-        <v>98</v>
+        <v>68</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D67" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="E67" s="5" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>67</v>
-      </c>
-      <c r="B68" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="C68" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="D68" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="E68" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="F68" t="s">
-        <v>121</v>
+        <v>69</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D68" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="E68" s="5">
+        <v>39</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>188</v>
+        <v>164</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="D69" s="4" t="s">
-        <v>220</v>
+        <v>183</v>
       </c>
       <c r="E69" s="5" t="s">
-        <v>14</v>
+        <v>93</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>189</v>
+        <v>165</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="D70" s="4" t="s">
-        <v>224</v>
-      </c>
-      <c r="E70" s="5">
-        <v>39</v>
+        <v>215</v>
+      </c>
+      <c r="E70" s="5" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>252</v>
+        <v>166</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>253</v>
+        <v>91</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>229</v>
+        <v>214</v>
       </c>
       <c r="E71" s="5" t="s">
-        <v>254</v>
+        <v>96</v>
+      </c>
+      <c r="F71" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>71</v>
-      </c>
-      <c r="B72" s="4" t="s">
-        <v>190</v>
-      </c>
-      <c r="C72" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="D72" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="E72" s="5" t="s">
-        <v>106</v>
+        <v>74</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="E72" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>72</v>
-      </c>
-      <c r="B73" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="C73" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="E73" s="3" t="s">
         <v>103</v>
-      </c>
-      <c r="D73" s="4" t="s">
-        <v>251</v>
-      </c>
-      <c r="E73" s="5" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>73</v>
-      </c>
-      <c r="B74" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="C74" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C74" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="D74" s="4" t="s">
-        <v>250</v>
-      </c>
-      <c r="E74" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="F74" t="s">
-        <v>121</v>
+      <c r="D74" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="E74" s="3" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>0</v>
+        <v>169</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>1</v>
+        <v>106</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>14</v>
+        <v>107</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>193</v>
+        <v>170</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>123</v>
+        <v>108</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>235</v>
+        <v>216</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77">
-        <v>76</v>
-      </c>
-      <c r="B77" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="C77" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="D77" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="E77" s="3" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78">
-        <v>77</v>
-      </c>
-      <c r="B78" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="C78" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="D78" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="E78" s="3" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79">
-        <v>78</v>
-      </c>
-      <c r="B79" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="C79" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="D79" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="E79" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="F79" t="s">
-        <v>121</v>
+        <v>109</v>
+      </c>
+      <c r="F76" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:E79" xr:uid="{16B76558-8B24-41A2-80CE-D2D9E66F99DE}"/>
+  <autoFilter ref="B1:E76" xr:uid="{16B76558-8B24-41A2-80CE-D2D9E66F99DE}"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2779,121 +2680,121 @@
   <sheetData>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>260</v>
+        <v>221</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>277</v>
+        <v>238</v>
       </c>
       <c r="B6" t="s">
-        <v>278</v>
+        <v>239</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>266</v>
+        <v>227</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>263</v>
+        <v>224</v>
       </c>
       <c r="B8" t="s">
-        <v>282</v>
+        <v>243</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>262</v>
+        <v>223</v>
       </c>
       <c r="B9" t="s">
-        <v>288</v>
+        <v>249</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>279</v>
+        <v>240</v>
       </c>
       <c r="B10" t="s">
-        <v>280</v>
+        <v>241</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>264</v>
+        <v>225</v>
       </c>
       <c r="B11" t="s">
-        <v>281</v>
+        <v>242</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>275</v>
+        <v>236</v>
       </c>
       <c r="B12" t="s">
-        <v>268</v>
+        <v>229</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>276</v>
+        <v>237</v>
       </c>
       <c r="B13" t="s">
-        <v>267</v>
+        <v>228</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>265</v>
+        <v>226</v>
       </c>
       <c r="B14" t="s">
-        <v>269</v>
+        <v>230</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>272</v>
+        <v>233</v>
       </c>
       <c r="B15" t="s">
-        <v>273</v>
+        <v>234</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>270</v>
+        <v>231</v>
       </c>
       <c r="B16" t="s">
-        <v>271</v>
+        <v>232</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>261</v>
+        <v>222</v>
       </c>
       <c r="B17" t="s">
-        <v>274</v>
+        <v>235</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>284</v>
+        <v>245</v>
       </c>
       <c r="B20" t="s">
-        <v>283</v>
+        <v>244</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>286</v>
+        <v>247</v>
       </c>
       <c r="B21" t="s">
-        <v>285</v>
+        <v>246</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>287</v>
+        <v>248</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Optimisation Structure. Delete units, ui-cards
</commit_message>
<xml_diff>
--- a/struct.xlsx
+++ b/struct.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Roman\Documents\Arduino\ESP32_HTTPS_OTA_APT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85D5FC58-87DA-4EB2-BC06-B143DD8E4124}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{801B47F9-786D-439A-8A4B-F9B791C7DB9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{40B8887A-0BD1-4A86-807F-5934227B243E}"/>
+    <workbookView xWindow="29235" yWindow="8880" windowWidth="17805" windowHeight="14760" xr2:uid="{40B8887A-0BD1-4A86-807F-5934227B243E}"/>
   </bookViews>
   <sheets>
     <sheet name="Struct" sheetId="2" r:id="rId1"/>
@@ -208,9 +208,6 @@
     <t>config.nodes.binary.pir.enabled</t>
   </si>
   <si>
-    <t>config.nodes.binary.pir.pin</t>
-  </si>
-  <si>
     <t>config.nodes.binary.pir.label</t>
   </si>
   <si>
@@ -232,9 +229,6 @@
     <t>config.nodes.binary.ld2420.enabled</t>
   </si>
   <si>
-    <t>config.nodes.binary.ld2420.pin</t>
-  </si>
-  <si>
     <t>config.nodes.binary.ld2420.label</t>
   </si>
   <si>
@@ -256,9 +250,6 @@
     <t>config.nodes.binary.door.enabled</t>
   </si>
   <si>
-    <t>config.nodes.binary.door.pin</t>
-  </si>
-  <si>
     <t>config.nodes.binary.door.type</t>
   </si>
   <si>
@@ -286,9 +277,6 @@
     <t>config.nodes.binary.flood.enabled</t>
   </si>
   <si>
-    <t>config.nodes.binary.flood.pin</t>
-  </si>
-  <si>
     <t>config.nodes.binary.flood.label</t>
   </si>
   <si>
@@ -310,9 +298,6 @@
     <t>config.nodes.analog.light_resistor.enabled</t>
   </si>
   <si>
-    <t>config.nodes.analog.light_resistor.pin</t>
-  </si>
-  <si>
     <t>config.nodes.analog.light_resistor.label</t>
   </si>
   <si>
@@ -631,9 +616,6 @@
     <t>int port</t>
   </si>
   <si>
-    <t>int pin</t>
-  </si>
-  <si>
     <t>"192.168.1.2"</t>
   </si>
   <si>
@@ -814,21 +796,9 @@
     <t>doc["bme_p"]</t>
   </si>
   <si>
-    <t>config.nodes.climate.bme280.pin</t>
-  </si>
-  <si>
     <t>doc["tcrt_p"]</t>
   </si>
   <si>
-    <t>config.nodes.climate.tcrt5000.pin</t>
-  </si>
-  <si>
-    <t>config.nodes.climate.dht22.pin</t>
-  </si>
-  <si>
-    <t>int</t>
-  </si>
-  <si>
     <t>21/22, "I2C"</t>
   </si>
   <si>
@@ -838,9 +808,6 @@
     <t>["°C","°C","°C","°C"]</t>
   </si>
   <si>
-    <t>config.nodes.climate.ds18b20.pin</t>
-  </si>
-  <si>
     <t>char unit[8]</t>
   </si>
   <si>
@@ -863,6 +830,39 @@
   </si>
   <si>
     <t>config.nodes.climate.tcrt5000.label</t>
+  </si>
+  <si>
+    <t>config.nodes.climate.bme280.pins</t>
+  </si>
+  <si>
+    <t>int pins[1]</t>
+  </si>
+  <si>
+    <t>[21] /22, "I2C"</t>
+  </si>
+  <si>
+    <t>config.nodes.climate.dht22.pins</t>
+  </si>
+  <si>
+    <t>config.nodes.climate.ds18b20.pins</t>
+  </si>
+  <si>
+    <t>config.nodes.binary.ld2420.pins</t>
+  </si>
+  <si>
+    <t>config.nodes.climate.tcrt5000.pins</t>
+  </si>
+  <si>
+    <t>config.nodes.binary.flood.pins</t>
+  </si>
+  <si>
+    <t>config.nodes.analog.light_resistor.pins</t>
+  </si>
+  <si>
+    <t>config.nodes.binary.pir.pins</t>
+  </si>
+  <si>
+    <t>config.nodes.binary.door.pins</t>
   </si>
 </sst>
 </file>
@@ -1298,8 +1298,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16B76558-8B24-41A2-80CE-D2D9E66F99DE}">
   <dimension ref="A1:F76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1320,10 +1320,10 @@
         <v>3</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1331,13 +1331,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>4</v>
@@ -1348,13 +1348,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="E3" s="3">
         <v>0</v>
@@ -1365,13 +1365,13 @@
         <v>12</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>14</v>
@@ -1382,16 +1382,16 @@
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1399,16 +1399,16 @@
         <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1416,19 +1416,19 @@
         <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>10</v>
       </c>
       <c r="F7" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1436,16 +1436,16 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1453,16 +1453,16 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1470,13 +1470,13 @@
         <v>8</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>14</v>
@@ -1487,16 +1487,16 @@
         <v>9</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1504,13 +1504,13 @@
         <v>10</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="E12" s="5">
         <v>0</v>
@@ -1521,13 +1521,13 @@
         <v>11</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>17</v>
@@ -1538,13 +1538,13 @@
         <v>12</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>14</v>
@@ -1555,16 +1555,16 @@
         <v>13</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>19</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1572,13 +1572,13 @@
         <v>14</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="E16" s="3">
         <v>1883</v>
@@ -1589,16 +1589,16 @@
         <v>15</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1606,16 +1606,16 @@
         <v>16</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -1623,19 +1623,19 @@
         <v>17</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>24</v>
       </c>
       <c r="F19" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1643,19 +1643,19 @@
         <v>18</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>25</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="E20" s="3">
         <v>5</v>
       </c>
       <c r="F20" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1663,13 +1663,13 @@
         <v>19</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>26</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>14</v>
@@ -1680,16 +1680,16 @@
         <v>20</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>256</v>
+        <v>262</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1697,13 +1697,13 @@
         <v>21</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>27</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>28</v>
@@ -1714,13 +1714,13 @@
         <v>22</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>29</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>30</v>
@@ -1731,13 +1731,13 @@
         <v>23</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>31</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>32</v>
@@ -1748,19 +1748,19 @@
         <v>24</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>33</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="E26" s="5" t="s">
         <v>34</v>
       </c>
       <c r="F26" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1768,13 +1768,13 @@
         <v>25</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>36</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>14</v>
@@ -1785,13 +1785,13 @@
         <v>26</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>195</v>
+        <v>263</v>
       </c>
       <c r="E28" s="3">
         <v>15</v>
@@ -1802,13 +1802,13 @@
         <v>27</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>37</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>38</v>
@@ -1819,13 +1819,13 @@
         <v>28</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>39</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>40</v>
@@ -1836,13 +1836,13 @@
         <v>29</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>41</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>42</v>
@@ -1853,19 +1853,19 @@
         <v>30</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>35</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>43</v>
       </c>
       <c r="F32" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1873,13 +1873,13 @@
         <v>31</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>45</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="E33" s="5" t="s">
         <v>14</v>
@@ -1890,13 +1890,13 @@
         <v>32</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>195</v>
+        <v>263</v>
       </c>
       <c r="E34" s="5">
         <v>4</v>
@@ -1907,19 +1907,19 @@
         <v>33</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="E35" s="5" t="s">
         <v>46</v>
       </c>
       <c r="F35" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -1927,13 +1927,13 @@
         <v>34</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>47</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="E36" s="5" t="s">
         <v>48</v>
@@ -1944,16 +1944,16 @@
         <v>35</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>49</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>262</v>
+        <v>252</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -1961,13 +1961,13 @@
         <v>36</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>50</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="E38" s="5" t="s">
         <v>51</v>
@@ -1978,19 +1978,19 @@
         <v>37</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>44</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="E39" s="5" t="s">
         <v>52</v>
       </c>
       <c r="F39" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -1998,13 +1998,13 @@
         <v>38</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>14</v>
@@ -2015,16 +2015,16 @@
         <v>39</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>258</v>
+        <v>268</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>261</v>
+        <v>251</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -2032,16 +2032,16 @@
         <v>40</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>272</v>
+        <v>261</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -2049,16 +2049,16 @@
         <v>41</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>266</v>
+        <v>255</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -2066,16 +2066,16 @@
         <v>42</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -2083,19 +2083,19 @@
         <v>43</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>270</v>
+        <v>259</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>268</v>
+        <v>257</v>
       </c>
       <c r="F45" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -2103,13 +2103,13 @@
         <v>44</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="C46" s="4" t="s">
         <v>53</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="E46" s="5" t="s">
         <v>14</v>
@@ -2120,13 +2120,13 @@
         <v>45</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>54</v>
+        <v>271</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>195</v>
+        <v>263</v>
       </c>
       <c r="E47" s="5">
         <v>35</v>
@@ -2137,16 +2137,16 @@
         <v>47</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C48" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="E48" s="5" t="s">
         <v>55</v>
-      </c>
-      <c r="D48" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="E48" s="5" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -2154,16 +2154,16 @@
         <v>48</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="C49" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="E49" s="5" t="s">
         <v>57</v>
-      </c>
-      <c r="D49" s="4" t="s">
-        <v>215</v>
-      </c>
-      <c r="E49" s="5" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -2171,19 +2171,19 @@
         <v>49</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="C50" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="E50" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D50" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="E50" s="5" t="s">
-        <v>60</v>
-      </c>
       <c r="F50" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -2191,13 +2191,13 @@
         <v>50</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>14</v>
@@ -2208,13 +2208,13 @@
         <v>51</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>62</v>
+        <v>267</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>195</v>
+        <v>263</v>
       </c>
       <c r="E52" s="3">
         <v>35</v>
@@ -2225,16 +2225,16 @@
         <v>53</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
@@ -2242,16 +2242,16 @@
         <v>54</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -2259,19 +2259,19 @@
         <v>55</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F55" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -2279,13 +2279,13 @@
         <v>56</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="E56" s="5" t="s">
         <v>14</v>
@@ -2296,13 +2296,13 @@
         <v>57</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>70</v>
+        <v>272</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>195</v>
+        <v>263</v>
       </c>
       <c r="E57" s="5">
         <v>36</v>
@@ -2313,16 +2313,16 @@
         <v>58</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="E58" s="5" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
@@ -2330,16 +2330,16 @@
         <v>59</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
@@ -2347,16 +2347,16 @@
         <v>60</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="E60" s="5" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
@@ -2364,19 +2364,19 @@
         <v>61</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="E61" s="5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F61" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
@@ -2384,13 +2384,13 @@
         <v>62</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="E62" s="3" t="s">
         <v>14</v>
@@ -2401,13 +2401,13 @@
         <v>63</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>80</v>
+        <v>269</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>195</v>
+        <v>263</v>
       </c>
       <c r="E63" s="3">
         <v>34</v>
@@ -2418,16 +2418,16 @@
         <v>65</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
@@ -2435,16 +2435,16 @@
         <v>66</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
@@ -2452,19 +2452,19 @@
         <v>67</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="F66" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
@@ -2472,13 +2472,13 @@
         <v>68</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="E67" s="5" t="s">
         <v>14</v>
@@ -2489,13 +2489,13 @@
         <v>69</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>88</v>
+        <v>270</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>195</v>
+        <v>263</v>
       </c>
       <c r="E68" s="5">
         <v>39</v>
@@ -2506,16 +2506,16 @@
         <v>71</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D69" s="4" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="E69" s="5" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
@@ -2523,16 +2523,16 @@
         <v>72</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D70" s="4" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="E70" s="5" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
@@ -2540,19 +2540,19 @@
         <v>73</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C71" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D71" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="E71" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="D71" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="E71" s="5" t="s">
-        <v>96</v>
-      </c>
       <c r="F71" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
@@ -2566,7 +2566,7 @@
         <v>1</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="E72" s="3" t="s">
         <v>14</v>
@@ -2577,16 +2577,16 @@
         <v>75</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
@@ -2594,16 +2594,16 @@
         <v>76</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
@@ -2611,16 +2611,16 @@
         <v>77</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
@@ -2628,19 +2628,19 @@
         <v>78</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="F76" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -2680,121 +2680,121 @@
   <sheetData>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="B6" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="B8" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="B9" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="B10" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="B11" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="B12" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="B13" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="B14" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="B15" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="B16" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="B17" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="B20" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="B21" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added option to work with MQTT
</commit_message>
<xml_diff>
--- a/struct.xlsx
+++ b/struct.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Roman\Documents\Arduino\ESP32_HTTPS_OTA_APT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{801B47F9-786D-439A-8A4B-F9B791C7DB9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B082BBC-777D-44F0-AA18-EB1F34F18EC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29235" yWindow="8880" windowWidth="17805" windowHeight="14760" xr2:uid="{40B8887A-0BD1-4A86-807F-5934227B243E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{40B8887A-0BD1-4A86-807F-5934227B243E}"/>
   </bookViews>
   <sheets>
     <sheet name="Struct" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="API" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Struct!$B$1:$E$76</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Struct!$B$1:$E$77</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="275">
   <si>
     <t>doc["r_en"]</t>
   </si>
@@ -517,21 +517,6 @@
     <t>doc["fl_t"]</t>
   </si>
   <si>
-    <t>doc["5516_en"]</t>
-  </si>
-  <si>
-    <t>doc["5516_p"]</t>
-  </si>
-  <si>
-    <t>doc["5516_l"]</t>
-  </si>
-  <si>
-    <t>doc["5516_c"]</t>
-  </si>
-  <si>
-    <t>doc["5516_t"]</t>
-  </si>
-  <si>
     <t>doc["r_p"]</t>
   </si>
   <si>
@@ -577,9 +562,6 @@
     <t>char user[32]</t>
   </si>
   <si>
-    <t>char host[32]</t>
-  </si>
-  <si>
     <t>char label[32]</t>
   </si>
   <si>
@@ -863,6 +845,30 @@
   </si>
   <si>
     <t>config.nodes.binary.door.pins</t>
+  </si>
+  <si>
+    <t>char host[64]</t>
+  </si>
+  <si>
+    <t>doc["m_id"]</t>
+  </si>
+  <si>
+    <t>config.services.mqtt.id</t>
+  </si>
+  <si>
+    <t>doc["lr_en"]</t>
+  </si>
+  <si>
+    <t>doc["lr_p"]</t>
+  </si>
+  <si>
+    <t>doc["lr_l"]</t>
+  </si>
+  <si>
+    <t>doc["lr_c"]</t>
+  </si>
+  <si>
+    <t>doc["lr_t"]</t>
   </si>
 </sst>
 </file>
@@ -1296,10 +1302,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16B76558-8B24-41A2-80CE-D2D9E66F99DE}">
-  <dimension ref="A1:F76"/>
+  <dimension ref="A1:F77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1320,7 +1326,7 @@
         <v>3</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>105</v>
@@ -1331,13 +1337,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>4</v>
@@ -1348,13 +1354,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="E3" s="3">
         <v>0</v>
@@ -1365,13 +1371,13 @@
         <v>12</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>14</v>
@@ -1382,16 +1388,16 @@
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1399,16 +1405,16 @@
         <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1416,13 +1422,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>10</v>
@@ -1436,16 +1442,16 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1453,16 +1459,16 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1476,7 +1482,7 @@
         <v>13</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>14</v>
@@ -1487,16 +1493,16 @@
         <v>9</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1504,13 +1510,13 @@
         <v>10</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>106</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="E12" s="5">
         <v>0</v>
@@ -1521,13 +1527,13 @@
         <v>11</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>17</v>
@@ -1544,7 +1550,7 @@
         <v>18</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>14</v>
@@ -1555,1096 +1561,1113 @@
         <v>13</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>109</v>
+        <v>268</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>19</v>
+        <v>269</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>177</v>
+        <v>267</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>190</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="E16" s="3">
-        <v>1883</v>
+        <v>267</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>191</v>
+        <v>183</v>
+      </c>
+      <c r="E17" s="3">
+        <v>1883</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>212</v>
+        <v>112</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>193</v>
+        <v>170</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F19" t="s">
-        <v>93</v>
+        <v>186</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>113</v>
+        <v>206</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="E20" s="3">
-        <v>5</v>
+        <v>187</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="F20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>19</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>14</v>
+        <v>18</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="E21" s="3">
+        <v>5</v>
+      </c>
+      <c r="F21" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>249</v>
+        <v>114</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>262</v>
+        <v>26</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>263</v>
+        <v>180</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>264</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>116</v>
+        <v>243</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>27</v>
+        <v>256</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>195</v>
+        <v>257</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>28</v>
+        <v>258</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F26" t="s">
-        <v>95</v>
+        <v>32</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>25</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>14</v>
+        <v>24</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F27" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>265</v>
+        <v>36</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="E28" s="3">
-        <v>15</v>
+        <v>180</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>37</v>
+        <v>259</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>38</v>
+        <v>257</v>
+      </c>
+      <c r="E29" s="3">
+        <v>15</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>201</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F32" t="s">
-        <v>95</v>
+        <v>42</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>31</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="E33" s="5" t="s">
-        <v>14</v>
+        <v>30</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F33" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>266</v>
+        <v>45</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>263</v>
-      </c>
-      <c r="E34" s="5">
-        <v>4</v>
+        <v>180</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>213</v>
+        <v>124</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>214</v>
+        <v>260</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>202</v>
-      </c>
-      <c r="E35" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="F35" t="s">
-        <v>96</v>
+        <v>257</v>
+      </c>
+      <c r="E35" s="5">
+        <v>4</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>125</v>
+        <v>207</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>47</v>
+        <v>208</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
+      </c>
+      <c r="F36" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>252</v>
+        <v>197</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>253</v>
+        <v>48</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>204</v>
+        <v>246</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>51</v>
+        <v>247</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="F39" t="s">
-        <v>95</v>
+        <v>51</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>38</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="E40" s="3" t="s">
-        <v>14</v>
+        <v>37</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F40" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>250</v>
+        <v>131</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>268</v>
+        <v>89</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>263</v>
+        <v>180</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>251</v>
+        <v>14</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>132</v>
+        <v>244</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>178</v>
+        <v>257</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>90</v>
+        <v>245</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>254</v>
+        <v>172</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>255</v>
+        <v>90</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>209</v>
+        <v>248</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>257</v>
-      </c>
-      <c r="F45" t="s">
-        <v>95</v>
+        <v>250</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>44</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="D46" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="E46" s="5" t="s">
-        <v>14</v>
+        <v>43</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="F46" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>271</v>
+        <v>53</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>263</v>
-      </c>
-      <c r="E47" s="5">
-        <v>35</v>
+        <v>180</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>54</v>
+        <v>265</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="E48" s="5" t="s">
-        <v>55</v>
+        <v>257</v>
+      </c>
+      <c r="E48" s="5">
+        <v>35</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>209</v>
+        <v>172</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="F50" t="s">
-        <v>95</v>
+        <v>57</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>50</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="E51" s="3" t="s">
-        <v>14</v>
+        <v>49</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="E51" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F51" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>267</v>
+        <v>60</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="E52" s="3">
-        <v>35</v>
+        <v>180</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>61</v>
+        <v>261</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="E53" s="3" t="s">
-        <v>64</v>
+        <v>257</v>
+      </c>
+      <c r="E53" s="3">
+        <v>35</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>209</v>
+        <v>172</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="F55" t="s">
-        <v>95</v>
+        <v>65</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>56</v>
-      </c>
-      <c r="B56" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="C56" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="D56" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="E56" s="5" t="s">
-        <v>14</v>
+        <v>55</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F56" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>272</v>
+        <v>67</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>263</v>
-      </c>
-      <c r="E57" s="5">
-        <v>36</v>
+        <v>180</v>
+      </c>
+      <c r="E57" s="5" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>68</v>
+        <v>266</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="E58" s="5" t="s">
-        <v>72</v>
+        <v>257</v>
+      </c>
+      <c r="E58" s="5">
+        <v>36</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>178</v>
+        <v>188</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>209</v>
+        <v>172</v>
       </c>
       <c r="E60" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="E61" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="F61" t="s">
-        <v>95</v>
+        <v>74</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>62</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D62" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="E62" s="3" t="s">
-        <v>14</v>
+        <v>61</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D62" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="E62" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="F62" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>269</v>
+        <v>76</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="E63" s="3">
-        <v>34</v>
+        <v>180</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>77</v>
+        <v>263</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="E64" s="3" t="s">
-        <v>80</v>
+        <v>257</v>
+      </c>
+      <c r="E64" s="3">
+        <v>34</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>209</v>
+        <v>172</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="F66" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>68</v>
-      </c>
-      <c r="B67" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="C67" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="D67" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="E67" s="5" t="s">
-        <v>14</v>
+        <v>67</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="E67" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F67" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>158</v>
+        <v>270</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>270</v>
+        <v>83</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>263</v>
-      </c>
-      <c r="E68" s="5">
-        <v>39</v>
+        <v>180</v>
+      </c>
+      <c r="E68" s="5" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>159</v>
+        <v>271</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>84</v>
+        <v>264</v>
       </c>
       <c r="D69" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="E69" s="5" t="s">
-        <v>88</v>
+        <v>257</v>
+      </c>
+      <c r="E69" s="5">
+        <v>39</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>160</v>
+        <v>272</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D70" s="4" t="s">
-        <v>209</v>
+        <v>172</v>
       </c>
       <c r="E70" s="5" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>161</v>
+        <v>273</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="E71" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="F71" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>74</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C72" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D72" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="E72" s="3" t="s">
-        <v>14</v>
+        <v>73</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D72" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="E72" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="F72" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>162</v>
+        <v>0</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>97</v>
+        <v>1</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>198</v>
+        <v>180</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>98</v>
+        <v>14</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76">
+        <v>77</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="E76" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77">
         <v>78</v>
       </c>
-      <c r="B76" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="C76" s="2" t="s">
+      <c r="B77" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C77" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="D76" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="E76" s="3" t="s">
+      <c r="D77" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="E77" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="F76" t="s">
+      <c r="F77" t="s">
         <v>95</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:E76" xr:uid="{16B76558-8B24-41A2-80CE-D2D9E66F99DE}"/>
+  <autoFilter ref="B1:E77" xr:uid="{16B76558-8B24-41A2-80CE-D2D9E66F99DE}"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2680,121 +2703,121 @@
   <sheetData>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="B6" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="B8" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="B9" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="B10" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="B11" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="B12" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="B13" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="B14" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="B15" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="B16" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="B17" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="B20" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="B21" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
     </row>
   </sheetData>

</xml_diff>